<commit_message>
mac Mie 28 Sep 2022 18:02:43 EEST
</commit_message>
<xml_diff>
--- a/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_august_2022_Alex_Bora.xlsx
+++ b/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_august_2022_Alex_Bora.xlsx
@@ -629,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>60476</v>
+        <v>63129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1057,7 +1057,7 @@
         <v>30</v>
       </c>
       <c r="B46" s="4">
-        <v>63129</v>
+        <v>65782</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">

</xml_diff>